<commit_message>
+ RC version for 2DF Convertor
</commit_message>
<xml_diff>
--- a/2DFireConvertor/template.xlsx
+++ b/2DFireConvertor/template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\NANLI_DEV\ZiiPOSMenuBuilder\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Nan_Dev\ZiiPOSMenuBuilder\2DFireConvertor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E143EE2-3CB1-4B0F-BE9C-D64E7D6B57E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D87326CE-2E1D-466E-AADA-B30B1927686D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="2" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MenuGroupTable" sheetId="2" r:id="rId1"/>
@@ -904,7 +904,7 @@
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection sqref="A1:H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1052,7 +1052,7 @@
   <dimension ref="A1:L1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:N37"/>
+      <selection activeCell="P33" sqref="P33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1148,7 +1148,7 @@
   <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G7" sqref="A2:G7"/>
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1186,8 +1186,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:AC2"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="R20" sqref="R20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O9" sqref="O9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1197,6 +1197,11 @@
     <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="7" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="20.28515625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="15.5703125" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="14.7109375" bestFit="1" customWidth="1"/>
@@ -1401,8 +1406,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:CX2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="CE1" workbookViewId="0">
-      <selection activeCell="CM2" sqref="CM2"/>
+    <sheetView topLeftCell="BY1" workbookViewId="0">
+      <selection activeCell="CH13" activeCellId="1" sqref="H1 CH13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>